<commit_message>
removed google analytics and updated privacy policy (no data is collected anymore)
</commit_message>
<xml_diff>
--- a/assets/pages/gwent/seasonal_stats.xlsx
+++ b/assets/pages/gwent/seasonal_stats.xlsx
@@ -1,37 +1,144 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+  <si>
+    <t>season</t>
+  </si>
+  <si>
+    <t>min_mmr</t>
+  </si>
+  <si>
+    <t>max_mmr</t>
+  </si>
+  <si>
+    <t>num_matches</t>
+  </si>
+  <si>
+    <t>top500_cutoff</t>
+  </si>
+  <si>
+    <t>top200_cutoff</t>
+  </si>
+  <si>
+    <t>top64_cutoff</t>
+  </si>
+  <si>
+    <t>M2_01 Wolf 2020</t>
+  </si>
+  <si>
+    <t>M2_02 Love 2020</t>
+  </si>
+  <si>
+    <t>M2_03 Bear 2020</t>
+  </si>
+  <si>
+    <t>M2_04 Elf 2020</t>
+  </si>
+  <si>
+    <t>M2_05 Viper 2020</t>
+  </si>
+  <si>
+    <t>M2_06 Magic 2020</t>
+  </si>
+  <si>
+    <t>M2_07 Griffin 2020</t>
+  </si>
+  <si>
+    <t>M2_08 Draconid 2020</t>
+  </si>
+  <si>
+    <t>M2_09 Dryad 2020</t>
+  </si>
+  <si>
+    <t>M2_10 Cat 2020</t>
+  </si>
+  <si>
+    <t>M2_11 Mahakam 2020</t>
+  </si>
+  <si>
+    <t>M2_12 Wild Hunt 2020</t>
+  </si>
+  <si>
+    <t>M3_01 Wolf 2021</t>
+  </si>
+  <si>
+    <t>M3_02 Love 2021</t>
+  </si>
+  <si>
+    <t>M3_03 Bear 2021</t>
+  </si>
+  <si>
+    <t>M3_04 Elf 2021</t>
+  </si>
+  <si>
+    <t>M3_05 Viper 2021</t>
+  </si>
+  <si>
+    <t>M3_06 Magic 2021</t>
+  </si>
+  <si>
+    <t>M3_07 Griffin 2021</t>
+  </si>
+  <si>
+    <t>M3_08 Draconid 2021</t>
+  </si>
+  <si>
+    <t>M3_09 Dryad 2021</t>
+  </si>
+  <si>
+    <t>M3_10 Cat 2021</t>
+  </si>
+  <si>
+    <t>M3_11 Mahakam 2021</t>
+  </si>
+  <si>
+    <t>M3_12 Wild Hunt 2021</t>
+  </si>
+  <si>
+    <t>M4_01 Wolf 2022</t>
+  </si>
+  <si>
+    <t>M4_02 Love 2022</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +153,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -420,757 +469,713 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>season</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>min_mmr</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>max_mmr</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>num_matches</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>top500_cutoff</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>top200_cutoff</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>top64_cutoff</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="1" spans="1:8">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>M2_01 Wolf 2020</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
         <v>2407</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>10484</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>699496</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>9749</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>9872</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>10061</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:8">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>M2_02 Love 2020</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
         <v>7776</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>10537</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>769172</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>9832</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>9952</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3">
         <v>10117</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>M2_03 Bear 2020</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
         <v>9427</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>10669</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>862283</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>9867</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>9995</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4">
         <v>10204</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>M2_04 Elf 2020</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
         <v>9666</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>10751</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>1004603</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>9952</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>10087</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H5">
         <v>10293</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>M2_05 Viper 2020</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
         <v>9635</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>10622</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>859640</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>9910</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>10028</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6">
         <v>10255</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>M2_06 Magic 2020</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
         <v>9624</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>10597</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>793013</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>9896</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>10002</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7">
         <v>10191</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:8">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>M2_07 Griffin 2020</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
         <v>9698</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>10667</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>996516</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8">
         <v>9978</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8">
         <v>10100</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H8">
         <v>10289</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:8">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>M2_08 Draconid 2020</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
         <v>9666</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>10546</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>837545</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9">
         <v>9946</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9">
         <v>10061</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H9">
         <v>10246</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:8">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>M2_09 Dryad 2020</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
         <v>9678</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>10725</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>854593</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10">
         <v>9946</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10">
         <v>10046</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H10">
         <v>10183</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:8">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>M2_10 Cat 2020</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
         <v>9703</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>10804</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
         <v>928845</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11">
         <v>9977</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G11">
         <v>10067</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H11">
         <v>10176</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:8">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>M2_11 Mahakam 2020</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
         <v>9706</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12">
         <v>10783</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12">
         <v>983150</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F12">
         <v>10000</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G12">
         <v>10090</v>
       </c>
-      <c r="H12" t="n">
+      <c r="H12">
         <v>10216</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:8">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>M2_12 Wild Hunt 2020</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
         <v>9756</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13">
         <v>10724</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13">
         <v>1182353</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F13">
         <v>10070</v>
       </c>
-      <c r="G13" t="n">
+      <c r="G13">
         <v>10172</v>
       </c>
-      <c r="H13" t="n">
+      <c r="H13">
         <v>10313</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:8">
+      <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>M3_01 Wolf 2021</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
         <v>9637</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14">
         <v>10653</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14">
         <v>808651</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F14">
         <v>9916</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G14">
         <v>10044</v>
       </c>
-      <c r="H14" t="n">
+      <c r="H14">
         <v>10295</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
+    <row r="15" spans="1:8">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>M3_02 Love 2021</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
         <v>9684</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15">
         <v>10714</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15">
         <v>917027</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F15">
         <v>9975</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G15">
         <v>10097</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H15">
         <v>10325</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
+    <row r="16" spans="1:8">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>M3_03 Bear 2021</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
         <v>9637</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16">
         <v>10576</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16">
         <v>766502</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F16">
         <v>9914</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G16">
         <v>10026</v>
       </c>
-      <c r="H16" t="n">
+      <c r="H16">
         <v>10230</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
+    <row r="17" spans="1:8">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>M3_04 Elf 2021</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17">
         <v>9686</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17">
         <v>10678</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17">
         <v>944323</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F17">
         <v>9992</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G17">
         <v>10102</v>
       </c>
-      <c r="H17" t="n">
+      <c r="H17">
         <v>10323</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
+    <row r="18" spans="1:8">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>M3_05 Viper 2021</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18">
         <v>9701</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18">
         <v>10753</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E18">
         <v>956484</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F18">
         <v>9998</v>
       </c>
-      <c r="G18" t="n">
+      <c r="G18">
         <v>10106</v>
       </c>
-      <c r="H18" t="n">
+      <c r="H18">
         <v>10300</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
+    <row r="19" spans="1:8">
+      <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>M3_06 Magic 2021</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
         <v>9681</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19">
         <v>10632</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E19">
         <v>869262</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F19">
         <v>9974</v>
       </c>
-      <c r="G19" t="n">
+      <c r="G19">
         <v>10082</v>
       </c>
-      <c r="H19" t="n">
+      <c r="H19">
         <v>10278</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
+    <row r="20" spans="1:8">
+      <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>M3_07 Griffin 2021</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20">
         <v>9669</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20">
         <v>10633</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E20">
         <v>856103</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F20">
         <v>9958</v>
       </c>
-      <c r="G20" t="n">
+      <c r="G20">
         <v>10067</v>
       </c>
-      <c r="H20" t="n">
+      <c r="H20">
         <v>10287</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
+    <row r="21" spans="1:8">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>M3_08 Draconid 2021</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21">
         <v>9681</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21">
         <v>10767</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21">
         <v>911273</v>
       </c>
-      <c r="F21" t="n">
+      <c r="F21">
         <v>9954</v>
       </c>
-      <c r="G21" t="n">
+      <c r="G21">
         <v>10079</v>
       </c>
-      <c r="H21" t="n">
+      <c r="H21">
         <v>10281</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
+    <row r="22" spans="1:8">
+      <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>M3_09 Dryad 2021</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22">
         <v>9688</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22">
         <v>10809</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E22">
         <v>940655</v>
       </c>
-      <c r="F22" t="n">
+      <c r="F22">
         <v>9968</v>
       </c>
-      <c r="G22" t="n">
+      <c r="G22">
         <v>10078</v>
       </c>
-      <c r="H22" t="n">
+      <c r="H22">
         <v>10250</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
+    <row r="23" spans="1:8">
+      <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>M3_10 Cat 2021</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23">
         <v>9614</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D23">
         <v>10366</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E23">
         <v>719696</v>
       </c>
-      <c r="F23" t="n">
+      <c r="F23">
         <v>9879</v>
       </c>
-      <c r="G23" t="n">
+      <c r="G23">
         <v>9974</v>
       </c>
-      <c r="H23" t="n">
+      <c r="H23">
         <v>10083</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
+    <row r="24" spans="1:8">
+      <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>M3_11 Mahakam 2021</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24">
         <v>9725</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24">
         <v>10580</v>
       </c>
-      <c r="E24" t="n">
+      <c r="E24">
         <v>1017256</v>
       </c>
-      <c r="F24" t="n">
+      <c r="F24">
         <v>10012</v>
       </c>
-      <c r="G24" t="n">
+      <c r="G24">
         <v>10122</v>
       </c>
-      <c r="H24" t="n">
+      <c r="H24">
         <v>10252</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
+    <row r="25" spans="1:8">
+      <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>M3_12 Wild Hunt 2021</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25">
         <v>9735</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D25">
         <v>10714</v>
       </c>
-      <c r="E25" t="n">
+      <c r="E25">
         <v>1044941</v>
       </c>
-      <c r="F25" t="n">
+      <c r="F25">
         <v>10032</v>
       </c>
-      <c r="G25" t="n">
+      <c r="G25">
         <v>10140</v>
       </c>
-      <c r="H25" t="n">
+      <c r="H25">
         <v>10271</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
+    <row r="26" spans="1:8">
+      <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>M4_01 Wolf 2022</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26">
         <v>9646</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D26">
         <v>10684</v>
       </c>
-      <c r="E26" t="n">
+      <c r="E26">
         <v>883881</v>
       </c>
-      <c r="F26" t="n">
+      <c r="F26">
         <v>9941</v>
       </c>
-      <c r="G26" t="n">
+      <c r="G26">
         <v>10093</v>
       </c>
-      <c r="H26" t="n">
+      <c r="H26">
         <v>10340</v>
       </c>
     </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27">
+        <v>9638</v>
+      </c>
+      <c r="D27">
+        <v>10652</v>
+      </c>
+      <c r="E27">
+        <v>852867</v>
+      </c>
+      <c r="F27">
+        <v>9932</v>
+      </c>
+      <c r="G27">
+        <v>10068</v>
+      </c>
+      <c r="H27">
+        <v>10312</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>